<commit_message>
Project Case54 is saved. v1 Type: SAVE.
</commit_message>
<xml_diff>
--- a/Case54/module1.xlsx
+++ b/Case54/module1.xlsx
@@ -3,28 +3,25 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ekosolapova/work/bugs/TestCasesEPBDS-8483/Case5/base/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ekosolapova/work/bugs/TestCasesEPBDS-8483/Case5/v1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{523783A0-CEC4-994E-8F6A-6B1F410F8519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F52683E-6B82-DD44-A6D0-FDCC19D1B5E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14700" yWindow="6240" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{ECDE2407-3746-D640-BF6D-E8EA64E98CEA}"/>
+    <workbookView xWindow="14700" yWindow="6240" windowWidth="28040" windowHeight="17440" xr2:uid="{ECDE2407-3746-D640-BF6D-E8EA64E98CEA}"/>
   </bookViews>
   <sheets>
     <sheet name="TheSheetHello Kitty" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <definedNames>
     <definedName name="uscodes">#REF!</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -101,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="79">
   <si>
     <t>Datatype MyDatatype</t>
   </si>
@@ -122,9 +119,6 @@
   </si>
   <si>
     <t>id</t>
-  </si>
-  <si>
-    <t>Data MyDatatypeData</t>
   </si>
   <si>
     <t>johndoe</t>
@@ -347,11 +341,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
-      <color theme="1" rgb="000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -359,14 +352,14 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color theme="1" rgb="000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
-      <color theme="1" rgb="000000"/>
+      <color theme="1"/>
       <name val="Monaco"/>
       <family val="2"/>
     </font>
@@ -420,7 +413,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485" rgb="4472C4"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -443,7 +436,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -642,20 +635,134 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -705,6 +812,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -720,19 +845,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="ForTest"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1032,148 +1144,149 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{308B9C1F-3537-9747-9E2A-F72A8C9A517D}">
-  <dimension ref="C7:F22"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16:F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C7" s="4" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="B1" s="35"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="34"/>
+    </row>
+    <row r="8" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A8" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="C8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A9" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="26">
         <v>1</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C9" s="1" t="s">
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="26">
         <v>2</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="28">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="26">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="B12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="28">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="29">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="3:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="C11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C16" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="3:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="C17" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="3:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="C18" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C19" s="1">
-        <v>1</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C20" s="1">
-        <v>2</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C21" s="1">
-        <v>3</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" s="1" t="s">
+      <c r="B13" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="F21" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C22" s="1">
-        <v>4</v>
-      </c>
-      <c r="D22" s="1" t="s">
+      <c r="C13" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F22" s="1">
+      <c r="D13" s="31">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1183,7 +1296,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B797EF6-3730-A549-AA02-8AA62FB94CD8}">
   <dimension ref="C6:U24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -1191,304 +1304,304 @@
   <sheetData>
     <row r="6" spans="3:21" x14ac:dyDescent="0.2">
       <c r="I6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="3:21" x14ac:dyDescent="0.2">
       <c r="I7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="O7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="P7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="Q7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="R7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="R7" s="1" t="s">
+      <c r="S7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="S7" s="1" t="s">
+      <c r="T7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="T7" s="1" t="s">
+      <c r="U7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="U7" s="1" t="s">
+    </row>
+    <row r="8" spans="3:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="3:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="5" t="s">
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="4"/>
+      <c r="I8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="6"/>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="M8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="N8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="O8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="P8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="Q8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="R8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="R8" s="1" t="s">
+      <c r="S8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="S8" s="1" t="s">
+      <c r="T8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="T8" s="1" t="s">
+      <c r="U8" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="U8" s="1" t="s">
+    </row>
+    <row r="9" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C9" s="5" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="9" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="C9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="E9" s="7"/>
+      <c r="F9" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="10" t="s">
+      <c r="I9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="L9" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="M9" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="N9" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="N9" s="1" t="s">
+      <c r="O9" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="P9" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="P9" s="1" t="s">
+      <c r="Q9" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="Q9" s="1" t="s">
+      <c r="R9" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="R9" s="1" t="s">
+      <c r="S9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="S9" s="1" t="s">
+      <c r="T9" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="T9" s="1" t="s">
+      <c r="U9" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="U9" s="1" t="s">
+    </row>
+    <row r="10" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C10" s="9"/>
+      <c r="D10" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="10" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="C10" s="11"/>
-      <c r="D10" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="12" t="s">
+    <row r="11" spans="3:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="11"/>
+      <c r="D11" s="12" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="11" spans="3:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="13"/>
-      <c r="D11" s="14" t="s">
+      <c r="E11" s="13"/>
+      <c r="F11" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="16" t="s">
+    </row>
+    <row r="12" spans="3:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="16" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="12" spans="3:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" s="18" t="s">
+      <c r="E12" s="17"/>
+      <c r="F12" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="E12" s="19"/>
-      <c r="F12" s="20" t="s">
+    </row>
+    <row r="13" spans="3:21" ht="146" x14ac:dyDescent="0.2">
+      <c r="C13" s="19" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="13" spans="3:21" ht="146" x14ac:dyDescent="0.2">
-      <c r="C13" s="21" t="s">
+      <c r="D13" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="E13" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="F13" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="E13" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="F13" s="23" t="s">
+    </row>
+    <row r="14" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C14" s="22"/>
+      <c r="D14" s="23" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="14" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="C14" s="24"/>
-      <c r="D14" s="25" t="s">
+      <c r="E14" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" s="24"/>
+    </row>
+    <row r="15" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C15" s="22"/>
+      <c r="D15" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="E14" s="25" t="s">
+      <c r="E15" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="F14" s="26"/>
-    </row>
-    <row r="15" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="C15" s="24"/>
-      <c r="D15" s="25" t="s">
+      <c r="F15" s="24"/>
+    </row>
+    <row r="16" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C16" s="22"/>
+      <c r="D16" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="25" t="s">
+      <c r="E16" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="F15" s="26"/>
-    </row>
-    <row r="16" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="C16" s="24"/>
-      <c r="D16" s="25" t="s">
+      <c r="F16" s="24"/>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C17" s="22"/>
+      <c r="D17" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="E16" s="25" t="s">
+      <c r="E17" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="F16" s="26"/>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C17" s="24"/>
-      <c r="D17" s="25" t="s">
+      <c r="F17" s="24"/>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C18" s="22"/>
+      <c r="D18" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="E17" s="25" t="s">
+      <c r="E18" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="F17" s="26"/>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C18" s="24"/>
-      <c r="D18" s="25" t="s">
+      <c r="F18" s="24"/>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C19" s="22"/>
+      <c r="D19" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="E18" s="25" t="s">
+      <c r="E19" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="F18" s="26"/>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C19" s="24"/>
-      <c r="D19" s="25" t="s">
+      <c r="F19" s="24"/>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C20" s="22"/>
+      <c r="D20" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="E19" s="25" t="s">
+      <c r="E20" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="F19" s="26"/>
-    </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C20" s="24"/>
-      <c r="D20" s="25" t="s">
+      <c r="F20" s="24"/>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C21" s="22"/>
+      <c r="D21" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="E20" s="25" t="s">
+      <c r="E21" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="F20" s="26"/>
-    </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C21" s="24"/>
-      <c r="D21" s="25" t="s">
+      <c r="F21" s="24"/>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C22" s="22"/>
+      <c r="D22" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="E21" s="25" t="s">
+      <c r="E22" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="F21" s="26"/>
-    </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C22" s="24"/>
-      <c r="D22" s="25" t="s">
+      <c r="F22" s="24"/>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C23" s="22"/>
+      <c r="D23" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="E22" s="25" t="s">
+      <c r="E23" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="F22" s="26"/>
-    </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C23" s="24"/>
-      <c r="D23" s="25" t="s">
+      <c r="F23" s="24"/>
+    </row>
+    <row r="24" spans="3:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="25"/>
+      <c r="D24" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="E23" s="25" t="s">
+      <c r="E24" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="F23" s="26"/>
-    </row>
-    <row r="24" spans="3:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="27"/>
-      <c r="D24" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="E24" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="F24" s="26"/>
+      <c r="F24" s="24"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>

<commit_message>
Restored from revision of lihfie lihewf on 01/23/2023 03:13:15 PM. Type: SAVE.
</commit_message>
<xml_diff>
--- a/Case54/module1.xlsx
+++ b/Case54/module1.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ekosolapova/work/bugs/TestCasesEPBDS-8483/Case5/base/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ekosolapova/work/bugs/TestCasesEPBDS-8483/Case5/v2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{523783A0-CEC4-994E-8F6A-6B1F410F8519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B1AA34-E5C3-B746-80C5-630E882DF6AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14700" yWindow="6240" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{ECDE2407-3746-D640-BF6D-E8EA64E98CEA}"/>
   </bookViews>
@@ -16,15 +16,12 @@
     <sheet name="TheSheetHello Kitty" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <definedNames>
     <definedName name="uscodes">#REF!</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -48,7 +45,7 @@
     <author>Stanislav Shor</author>
   </authors>
   <commentList>
-    <comment ref="D11" authorId="0" shapeId="0" xr:uid="{A7CD8C51-1D51-494B-89D4-A5911B975EB8}">
+    <comment ref="D23" authorId="0" shapeId="0" xr:uid="{A7CD8C51-1D51-494B-89D4-A5911B975EB8}">
       <text>
         <r>
           <rPr>
@@ -64,7 +61,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D13" authorId="0" shapeId="0" xr:uid="{22664757-042D-B448-A673-2D7333BCB63E}">
+    <comment ref="D25" authorId="0" shapeId="0" xr:uid="{22664757-042D-B448-A673-2D7333BCB63E}">
       <text>
         <r>
           <rPr>
@@ -80,18 +77,50 @@
         </r>
       </text>
     </comment>
-    <comment ref="E13" authorId="0" shapeId="0" xr:uid="{BE8E3FD1-8DFC-664E-A291-F43F65F03EE0}">
+    <comment ref="E25" authorId="0" shapeId="0" xr:uid="{BE8E3FD1-8DFC-664E-A291-F43F65F03EE0}">
       <text>
         <r>
           <rPr>
             <sz val="8"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
             <charset val="204"/>
           </rPr>
           <t xml:space="preserve">Notice using of combobox to select state abbrevs. Use Data|Validation|List Excel menu for this purpose. 
-This is yet another example in favor of using Excel as IDE
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">This is yet another example in favor of using Excel as IDE
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve"> 
 </t>
         </r>
       </text>
@@ -101,7 +130,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="81">
   <si>
     <t>Datatype MyDatatype</t>
   </si>
@@ -124,9 +153,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>Data MyDatatypeData</t>
-  </si>
-  <si>
     <t>johndoe</t>
   </si>
   <si>
@@ -341,17 +367,22 @@
   </si>
   <si>
     <t>Data MyDatatype Data</t>
+  </si>
+  <si>
+    <t>AA</t>
+  </si>
+  <si>
+    <t>BB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
-      <color theme="1" rgb="000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -359,14 +390,14 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color theme="1" rgb="000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
-      <color theme="1" rgb="000000"/>
+      <color theme="1"/>
       <name val="Monaco"/>
       <family val="2"/>
     </font>
@@ -410,8 +441,15 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -420,7 +458,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485" rgb="4472C4"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -442,6 +480,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="16">
     <border>
@@ -644,18 +694,12 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -680,7 +724,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -705,6 +748,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -720,19 +772,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="ForTest"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1035,16 +1074,16 @@
   <dimension ref="C7:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16:F16"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="7" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="4"/>
+      <c r="D7" s="29"/>
     </row>
     <row r="8" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C8" s="1" t="s">
@@ -1079,12 +1118,12 @@
       </c>
     </row>
     <row r="16" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C16" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
+      <c r="C16" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
     </row>
     <row r="17" spans="3:6" ht="19" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
@@ -1119,10 +1158,10 @@
         <v>1</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="F19" s="1">
         <v>10</v>
@@ -1133,10 +1172,10 @@
         <v>2</v>
       </c>
       <c r="D20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="F20" s="1">
         <v>11</v>
@@ -1147,10 +1186,10 @@
         <v>3</v>
       </c>
       <c r="D21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="F21" s="1">
         <v>9</v>
@@ -1161,10 +1200,10 @@
         <v>4</v>
       </c>
       <c r="D22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="F22" s="1">
         <v>8</v>
@@ -1181,318 +1220,343 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B797EF6-3730-A549-AA02-8AA62FB94CD8}">
-  <dimension ref="C6:U24"/>
+  <dimension ref="C6:O37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25:C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="6" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="I6" s="1" t="s">
+    <row r="6" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C6" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="25"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+    </row>
+    <row r="7" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C7" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="I7" s="1" t="s">
+      <c r="D7" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="E7" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="F7" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="G7" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="H7" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="I7" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="J7" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="K7" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="L7" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="R7" s="1" t="s">
+      <c r="M7" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="S7" s="1" t="s">
+      <c r="N7" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="T7" s="1" t="s">
+      <c r="O7" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="U7" s="1" t="s">
+    </row>
+    <row r="8" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C8" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="J8" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="K8" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="L8" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="M8" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="N8" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="O8" s="25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C9" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="I9" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="J9" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="K9" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="L9" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="M9" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="N9" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="O9" s="25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="3:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="6"/>
-      <c r="I8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="S8" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="T8" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="U8" s="1" t="s">
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C21" s="5" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="9" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="C9" s="7" t="s">
+      <c r="D21" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="E21" s="7"/>
+      <c r="F21" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q9" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="R9" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="T9" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="U9" s="1" t="s">
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C22" s="9"/>
+      <c r="D22" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E22" s="7"/>
+      <c r="F22" s="10" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="C10" s="11"/>
-      <c r="D10" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="12" t="s">
+    <row r="23" spans="3:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="11"/>
+      <c r="D23" s="12" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="11" spans="3:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="13"/>
-      <c r="D11" s="14" t="s">
+      <c r="E23" s="13"/>
+      <c r="F23" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="16" t="s">
+    </row>
+    <row r="24" spans="3:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="15" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="12" spans="3:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" s="18" t="s">
+      <c r="E24" s="16"/>
+      <c r="F24" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="E12" s="19"/>
-      <c r="F12" s="20" t="s">
+    </row>
+    <row r="25" spans="3:6" ht="146" x14ac:dyDescent="0.2">
+      <c r="C25" s="18" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="13" spans="3:21" ht="146" x14ac:dyDescent="0.2">
-      <c r="C13" s="21" t="s">
+      <c r="D25" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="E25" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="F25" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="E13" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="F13" s="23" t="s">
+    </row>
+    <row r="26" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C26" s="21"/>
+      <c r="D26" s="22" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="14" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="C14" s="24"/>
-      <c r="D14" s="25" t="s">
+      <c r="E26" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="F26" s="23"/>
+    </row>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C27" s="21"/>
+      <c r="D27" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="E14" s="25" t="s">
+      <c r="E27" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="F14" s="26"/>
-    </row>
-    <row r="15" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="C15" s="24"/>
-      <c r="D15" s="25" t="s">
+      <c r="F27" s="23"/>
+    </row>
+    <row r="28" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C28" s="21"/>
+      <c r="D28" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="25" t="s">
+      <c r="E28" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="F15" s="26"/>
-    </row>
-    <row r="16" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="C16" s="24"/>
-      <c r="D16" s="25" t="s">
+      <c r="F28" s="23"/>
+    </row>
+    <row r="29" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C29" s="21"/>
+      <c r="D29" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="E16" s="25" t="s">
+      <c r="E29" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="F16" s="26"/>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C17" s="24"/>
-      <c r="D17" s="25" t="s">
+      <c r="F29" s="23"/>
+    </row>
+    <row r="30" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C30" s="21"/>
+      <c r="D30" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="E17" s="25" t="s">
+      <c r="E30" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="F17" s="26"/>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C18" s="24"/>
-      <c r="D18" s="25" t="s">
+      <c r="F30" s="23"/>
+    </row>
+    <row r="31" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C31" s="21"/>
+      <c r="D31" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="E18" s="25" t="s">
+      <c r="E31" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="F18" s="26"/>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C19" s="24"/>
-      <c r="D19" s="25" t="s">
+      <c r="F31" s="23"/>
+    </row>
+    <row r="32" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C32" s="21"/>
+      <c r="D32" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="E19" s="25" t="s">
+      <c r="E32" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="F19" s="26"/>
-    </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C20" s="24"/>
-      <c r="D20" s="25" t="s">
+      <c r="F32" s="23"/>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C33" s="21"/>
+      <c r="D33" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="E20" s="25" t="s">
+      <c r="E33" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="F20" s="26"/>
-    </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C21" s="24"/>
-      <c r="D21" s="25" t="s">
+      <c r="F33" s="23"/>
+    </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C34" s="21"/>
+      <c r="D34" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="E21" s="25" t="s">
+      <c r="E34" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="F21" s="26"/>
-    </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C22" s="24"/>
-      <c r="D22" s="25" t="s">
+      <c r="F34" s="23"/>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C35" s="21"/>
+      <c r="D35" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="E22" s="25" t="s">
+      <c r="E35" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="F22" s="26"/>
-    </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C23" s="24"/>
-      <c r="D23" s="25" t="s">
+      <c r="F35" s="23"/>
+    </row>
+    <row r="36" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C36" s="21"/>
+      <c r="D36" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="E23" s="25" t="s">
+      <c r="E36" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="F23" s="26"/>
-    </row>
-    <row r="24" spans="3:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="27"/>
-      <c r="D24" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="E24" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="F24" s="26"/>
+      <c r="F36" s="23"/>
+    </row>
+    <row r="37" spans="3:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C37" s="24"/>
+      <c r="D37" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="E37" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="F37" s="23"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D13:E24" xr:uid="{75B242DE-8AA9-0049-8D52-DFC908ADB409}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D25:E37" xr:uid="{75B242DE-8AA9-0049-8D52-DFC908ADB409}">
       <formula1>uscodes</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>